<commit_message>
fix run without testdata file
</commit_message>
<xml_diff>
--- a/Data/EPD/DataFile.xlsx
+++ b/Data/EPD/DataFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E804FDBF-030D-4517-8B99-FEEC8DB4C77F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3049D746-1299-46D5-B1F1-6BA1C9708551}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Behandeling" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Type</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Polisnummer</t>
+  </si>
+  <si>
+    <t>Radiologie</t>
+  </si>
+  <si>
+    <t>Laag</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +494,32 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -497,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF867A2-5BD9-4131-9A86-BBAA89CA73B4}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
speed up select elements
</commit_message>
<xml_diff>
--- a/Data/EPD/DataFile.xlsx
+++ b/Data/EPD/DataFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3049D746-1299-46D5-B1F1-6BA1C9708551}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A69BA4-4F0E-4173-8167-F0AE1148A1B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +473,10 @@
         <v>18</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>

</xml_diff>